<commit_message>
Nuevo ETL Tareas + Ubicaciones
</commit_message>
<xml_diff>
--- a/data/Limpia/eliminados_filtrado_horario.xlsx
+++ b/data/Limpia/eliminados_filtrado_horario.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2988" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3018" uniqueCount="1014">
   <si>
     <t>Indice</t>
   </si>
@@ -3026,6 +3026,36 @@
   </si>
   <si>
     <t>34.766382S,55.736052W</t>
+  </si>
+  <si>
+    <t>34.771120S,55.758045W</t>
+  </si>
+  <si>
+    <t>34.771959S,55.761222W</t>
+  </si>
+  <si>
+    <t>34.772634S,55.761827W</t>
+  </si>
+  <si>
+    <t>34.768857S,55.769612W</t>
+  </si>
+  <si>
+    <t>34.768864S,55.770267W</t>
+  </si>
+  <si>
+    <t>34.766382S,55.736087W</t>
+  </si>
+  <si>
+    <t>34.766435S,55.736254W</t>
+  </si>
+  <si>
+    <t>34.764818S,55.752244W</t>
+  </si>
+  <si>
+    <t>34.764902S,55.752482W</t>
+  </si>
+  <si>
+    <t>34.766450S,55.736050W</t>
   </si>
 </sst>
 </file>
@@ -3387,7 +3417,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I994"/>
+  <dimension ref="A1:I1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -32219,6 +32249,296 @@
         <v>-55.736052</v>
       </c>
     </row>
+    <row r="995" spans="1:9">
+      <c r="A995">
+        <v>621</v>
+      </c>
+      <c r="B995" t="s">
+        <v>9</v>
+      </c>
+      <c r="C995" t="s">
+        <v>13</v>
+      </c>
+      <c r="D995" s="2">
+        <v>45699.77126157407</v>
+      </c>
+      <c r="E995" s="2">
+        <v>45699.77284722222</v>
+      </c>
+      <c r="F995">
+        <v>2.28</v>
+      </c>
+      <c r="G995" t="s">
+        <v>1004</v>
+      </c>
+      <c r="H995">
+        <v>-34.77112</v>
+      </c>
+      <c r="I995">
+        <v>-55.758045</v>
+      </c>
+    </row>
+    <row r="996" spans="1:9">
+      <c r="A996">
+        <v>622</v>
+      </c>
+      <c r="B996" t="s">
+        <v>9</v>
+      </c>
+      <c r="C996" t="s">
+        <v>14</v>
+      </c>
+      <c r="D996" s="2">
+        <v>45699.77284722222</v>
+      </c>
+      <c r="E996" s="2">
+        <v>45699.7825</v>
+      </c>
+      <c r="F996">
+        <v>13.9</v>
+      </c>
+      <c r="G996" t="s">
+        <v>1005</v>
+      </c>
+      <c r="H996">
+        <v>-34.771959</v>
+      </c>
+      <c r="I996">
+        <v>-55.761222</v>
+      </c>
+    </row>
+    <row r="997" spans="1:9">
+      <c r="A997">
+        <v>623</v>
+      </c>
+      <c r="B997" t="s">
+        <v>9</v>
+      </c>
+      <c r="C997" t="s">
+        <v>13</v>
+      </c>
+      <c r="D997" s="2">
+        <v>45699.7825</v>
+      </c>
+      <c r="E997" s="2">
+        <v>45699.78416666666</v>
+      </c>
+      <c r="F997">
+        <v>2.4</v>
+      </c>
+      <c r="G997" t="s">
+        <v>1006</v>
+      </c>
+      <c r="H997">
+        <v>-34.772634</v>
+      </c>
+      <c r="I997">
+        <v>-55.761827</v>
+      </c>
+    </row>
+    <row r="998" spans="1:9">
+      <c r="A998">
+        <v>624</v>
+      </c>
+      <c r="B998" t="s">
+        <v>9</v>
+      </c>
+      <c r="C998" t="s">
+        <v>14</v>
+      </c>
+      <c r="D998" s="2">
+        <v>45699.78416666666</v>
+      </c>
+      <c r="E998" s="2">
+        <v>45699.80545138889</v>
+      </c>
+      <c r="F998">
+        <v>30.65</v>
+      </c>
+      <c r="G998" t="s">
+        <v>1007</v>
+      </c>
+      <c r="H998">
+        <v>-34.768857</v>
+      </c>
+      <c r="I998">
+        <v>-55.769612</v>
+      </c>
+    </row>
+    <row r="999" spans="1:9">
+      <c r="A999">
+        <v>625</v>
+      </c>
+      <c r="B999" t="s">
+        <v>9</v>
+      </c>
+      <c r="C999" t="s">
+        <v>13</v>
+      </c>
+      <c r="D999" s="2">
+        <v>45699.80545138889</v>
+      </c>
+      <c r="E999" s="2">
+        <v>45699.81300925926</v>
+      </c>
+      <c r="F999">
+        <v>10.88</v>
+      </c>
+      <c r="G999" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H999">
+        <v>-34.768864</v>
+      </c>
+      <c r="I999">
+        <v>-55.770267</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:9">
+      <c r="A1000">
+        <v>626</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1000" s="2">
+        <v>45699.81300925926</v>
+      </c>
+      <c r="E1000" s="2">
+        <v>45699.85653935185</v>
+      </c>
+      <c r="F1000">
+        <v>62.68</v>
+      </c>
+      <c r="G1000" t="s">
+        <v>1009</v>
+      </c>
+      <c r="H1000">
+        <v>-34.766382</v>
+      </c>
+      <c r="I1000">
+        <v>-55.736087</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:9">
+      <c r="A1001">
+        <v>627</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1001" s="2">
+        <v>45699.85653935185</v>
+      </c>
+      <c r="E1001" s="2">
+        <v>45699.85959490741</v>
+      </c>
+      <c r="F1001">
+        <v>4.4</v>
+      </c>
+      <c r="G1001" t="s">
+        <v>1010</v>
+      </c>
+      <c r="H1001">
+        <v>-34.766435</v>
+      </c>
+      <c r="I1001">
+        <v>-55.736254</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:9">
+      <c r="A1002">
+        <v>628</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1002" s="2">
+        <v>45699.85959490741</v>
+      </c>
+      <c r="E1002" s="2">
+        <v>45699.91097222222</v>
+      </c>
+      <c r="F1002">
+        <v>73.98</v>
+      </c>
+      <c r="G1002" t="s">
+        <v>1011</v>
+      </c>
+      <c r="H1002">
+        <v>-34.764818</v>
+      </c>
+      <c r="I1002">
+        <v>-55.752244</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9">
+      <c r="A1003">
+        <v>629</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1003" s="2">
+        <v>45699.91097222222</v>
+      </c>
+      <c r="E1003" s="2">
+        <v>45699.91533564815</v>
+      </c>
+      <c r="F1003">
+        <v>6.28</v>
+      </c>
+      <c r="G1003" t="s">
+        <v>1012</v>
+      </c>
+      <c r="H1003">
+        <v>-34.764902</v>
+      </c>
+      <c r="I1003">
+        <v>-55.752482</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:9">
+      <c r="A1004">
+        <v>630</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1004" s="2">
+        <v>45699.91533564815</v>
+      </c>
+      <c r="E1004" s="2">
+        <v>45700.3089699074</v>
+      </c>
+      <c r="F1004">
+        <v>566.83</v>
+      </c>
+      <c r="G1004" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H1004">
+        <v>-34.76645</v>
+      </c>
+      <c r="I1004">
+        <v>-55.73605</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>